<commit_message>
Fixed diesel + wind issues
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{384EF942-1BB3-4AF5-A4C8-1EAD5F73D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA497DCF-02B6-4151-9C4F-709956496BB4}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{384EF942-1BB3-4AF5-A4C8-1EAD5F73D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0A33E09-9FCF-4848-BC50-36728E922D67}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="123">
   <si>
     <t>Unit</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>heat_recovery</t>
-  </si>
-  <si>
-    <t>jetfuel</t>
   </si>
 </sst>
 </file>
@@ -1231,9 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1505,9 +1500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478C130-C296-4571-ABF4-62E91E9E2767}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1727,7 +1720,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Fixed column name error
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel_4_InOutputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{384EF942-1BB3-4AF5-A4C8-1EAD5F73D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0A33E09-9FCF-4848-BC50-36728E922D67}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{384EF942-1BB3-4AF5-A4C8-1EAD5F73D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC212C26-504D-49D3-AB64-85014F02923E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -403,12 +403,6 @@
     <t>Relation_In1_In2</t>
   </si>
   <si>
-    <t>Relation_In1_In22</t>
-  </si>
-  <si>
-    <t>Relation_In1_In23</t>
-  </si>
-  <si>
     <t>Input3</t>
   </si>
   <si>
@@ -443,6 +437,12 @@
   </si>
   <si>
     <t>heat_recovery</t>
+  </si>
+  <si>
+    <t>Relation_In1_In3</t>
+  </si>
+  <si>
+    <t>Relation_In1_In4</t>
   </si>
 </sst>
 </file>
@@ -807,6 +807,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0333CFC6-D067-4B12-B0A1-83E429D32CCD}" name="Table1" displayName="Table1" ref="A1:R14" totalsRowShown="0">
   <autoFilter ref="A1:R14" xr:uid="{0333CFC6-D067-4B12-B0A1-83E429D32CCD}"/>
@@ -849,8 +853,8 @@
     <tableColumn id="15" xr3:uid="{E758FC30-F120-4234-A984-DD9BB9F5CBE5}" name="Output3" dataDxfId="10"/>
     <tableColumn id="16" xr3:uid="{85570B5D-60DB-4C61-80EB-881EDB346388}" name="Output4" dataDxfId="9"/>
     <tableColumn id="10" xr3:uid="{40961C24-C288-48FE-96C9-C696058F1146}" name="Relation_In1_In2" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E93572D0-6388-4D7C-A2BF-3805225F4F50}" name="Relation_In1_In22" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{BAF59A78-842A-475C-B900-52E45F0F2C02}" name="Relation_In1_In23" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E93572D0-6388-4D7C-A2BF-3805225F4F50}" name="Relation_In1_In3" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{BAF59A78-842A-475C-B900-52E45F0F2C02}" name="Relation_In1_In4" dataDxfId="6"/>
     <tableColumn id="11" xr3:uid="{63A0B53D-07BC-4C95-B97C-243557E4A128}" name="Relation_In_Out" dataDxfId="5"/>
     <tableColumn id="25" xr3:uid="{44B35FDD-04C5-401A-9765-766FCD023027}" name="Relation_Out1_Out2" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{3E00680F-559F-4DED-989F-C435D3C0AEC7}" name="Relation_Out1_Out22" dataDxfId="3"/>
@@ -1228,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1244,7 +1248,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
         <v>37</v>
@@ -1253,16 +1257,16 @@
         <v>33</v>
       </c>
       <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>119</v>
       </c>
       <c r="J1" t="s">
         <v>88</v>
@@ -1280,7 +1284,7 @@
         <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P1" t="s">
         <v>39</v>
@@ -1426,7 +1430,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>95</v>
@@ -1473,7 +1477,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>95</v>
@@ -1500,7 +1504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478C130-C296-4571-ABF4-62E91E9E2767}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1522,10 +1528,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1534,19 +1540,19 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K1" t="s">
         <v>108</v>
       </c>
       <c r="L1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="M1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
@@ -1790,7 +1796,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>66</v>
@@ -1910,7 +1916,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>95</v>
@@ -1922,7 +1928,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1939,7 +1945,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>95</v>
@@ -1951,7 +1957,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>

</xml_diff>